<commit_message>
Change header to Device Name
</commit_message>
<xml_diff>
--- a/information/2025-Projector-Refresh-Import-Header-ForScripting-Subset.xlsx
+++ b/information/2025-Projector-Refresh-Import-Header-ForScripting-Subset.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbartolo\GitHub\HayesTicketCreator\information\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A712D806-41F7-4EA8-A656-153DD68ABEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="5325" yWindow="5325" windowWidth="57600" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Projector Name</t>
-  </si>
-  <si>
     <t>Tag</t>
   </si>
   <si>
@@ -25,50 +31,55 @@
     <t>IP Address</t>
   </si>
   <si>
-    <t>BUR-RM01-PROJ</t>
-  </si>
-  <si>
     <t>XCAX4801241</t>
   </si>
   <si>
     <t>10.20.131.31</t>
   </si>
   <si>
-    <t>BUR-RM02-PROJ</t>
-  </si>
-  <si>
     <t>XCAX4801236</t>
   </si>
   <si>
     <t>10.20.131.32</t>
   </si>
   <si>
-    <t>BUR-RM03-PROJ</t>
-  </si>
-  <si>
     <t>XCAX4801202</t>
   </si>
   <si>
     <t>10.20.131.33</t>
+  </si>
+  <si>
+    <t>TEST-RM01-PROJ</t>
+  </si>
+  <si>
+    <t>TEST-RM02-PROJ</t>
+  </si>
+  <si>
+    <t>TEST-RM03-PROJ</t>
+  </si>
+  <si>
+    <t>Device Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -78,45 +89,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -306,657 +320,660 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.88"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>769452</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>769452.0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>769453</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>769454</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
-        <v>769453.0</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3">
-        <v>769454.0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="3"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="3"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="3"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="3"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="3"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="3"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="3"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="3"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="3"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
       <c r="B98" s="3"/>
       <c r="C98" s="4"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
     </row>
-    <row r="100">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
       <c r="B100" s="3"/>
       <c r="C100" s="4"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="3"/>
       <c r="C101" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>